<commit_message>
Localisation levers controlled from SATIM scens
</commit_message>
<xml_diff>
--- a/VT_REGION1_LABMATACT.xlsx
+++ b/VT_REGION1_LABMATACT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4265139D-E14A-4414-BC52-A006B73E2348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1267114-0498-4DCE-A1FC-D54F6FFE9419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="-17400" windowWidth="28770" windowHeight="15570" xr2:uid="{42DD4C14-1DB9-4C61-AA3D-EE41BBDB568D}"/>
+    <workbookView xWindow="30" yWindow="630" windowWidth="28770" windowHeight="15570" xr2:uid="{42DD4C14-1DB9-4C61-AA3D-EE41BBDB568D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -339,6 +339,11 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
@@ -718,10 +723,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969F05AD-0ADD-4D58-8BDF-3FCA38EA7081}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C2:V40"/>
+  <dimension ref="C2:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47:L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,6 +1567,30 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
+      <c r="J23" t="str">
+        <f>"IMP"&amp;J5</f>
+        <v>IMPccons_e</v>
+      </c>
+      <c r="K23" s="14" t="str">
+        <f>"Imports of "&amp;K5</f>
+        <v>Imports of Construction</v>
+      </c>
+      <c r="L23" t="str">
+        <f>L18</f>
+        <v>Kt</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" ref="M23:O23" si="2">M18</f>
+        <v>Kt/a</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="2"/>
+        <v>ANNUAL</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="2"/>
+        <v>XTRACT,PRW</v>
+      </c>
       <c r="Q23" t="str">
         <f t="shared" si="0"/>
         <v>MINMATCOP</v>
@@ -1584,6 +1613,30 @@
       </c>
     </row>
     <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="J24" t="str">
+        <f t="shared" ref="J24:J27" si="3">"IMP"&amp;J6</f>
+        <v>IMPcmach_e</v>
+      </c>
+      <c r="K24" s="14" t="str">
+        <f t="shared" ref="K24:K27" si="4">"Imports of "&amp;K6</f>
+        <v>Imports of Machinery</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" ref="L24:O24" si="5">L19</f>
+        <v>Kt</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="5"/>
+        <v>Kt/a</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="5"/>
+        <v>ANNUAL</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="5"/>
+        <v>XTRACT,PRW</v>
+      </c>
       <c r="Q24" t="str">
         <f t="shared" si="0"/>
         <v>MINMATNIC</v>
@@ -1606,6 +1659,30 @@
       </c>
     </row>
     <row r="25" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="J25" t="str">
+        <f t="shared" si="3"/>
+        <v>IMPcemch_e</v>
+      </c>
+      <c r="K25" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>Imports of Electrical Machinery</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" ref="L25:O25" si="6">L20</f>
+        <v>Kt</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="6"/>
+        <v>Kt/a</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="6"/>
+        <v>ANNUAL</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="6"/>
+        <v>XTRACT,PRW</v>
+      </c>
       <c r="Q25" t="str">
         <f t="shared" si="0"/>
         <v>MINMATMNG</v>
@@ -1628,6 +1705,30 @@
       </c>
     </row>
     <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="J26" t="str">
+        <f t="shared" si="3"/>
+        <v>IMPcmetp</v>
+      </c>
+      <c r="K26" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>Imports of Metal Products</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" ref="L26:O26" si="7">L21</f>
+        <v>Kt</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="7"/>
+        <v>Kt/a</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="7"/>
+        <v>ANNUAL</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="7"/>
+        <v>XTRACT,PRW</v>
+      </c>
       <c r="Q26" t="str">
         <f t="shared" si="0"/>
         <v>MINMATCOB</v>
@@ -1650,6 +1751,30 @@
       </c>
     </row>
     <row r="27" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="J27" t="str">
+        <f t="shared" si="3"/>
+        <v>IMPcbsrv</v>
+      </c>
+      <c r="K27" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>Imports of Business Services</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" ref="L27:O27" si="8">L22</f>
+        <v>Kt</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="8"/>
+        <v>Kt/a</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="8"/>
+        <v>ANNUAL</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="8"/>
+        <v>XTRACT,PRW</v>
+      </c>
       <c r="Q27" t="str">
         <f>"MIN"&amp;Q14</f>
         <v>MINMATSIL</v>
@@ -1671,330 +1796,395 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="9" t="s">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="9" t="s">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="9" t="s">
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="3:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="C30" s="9" t="s">
+    <row r="36" spans="3:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E36" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="J30" s="9" t="s">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="J36" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K36" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L30" s="9" t="s">
+      <c r="L36" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="9" t="s">
+      <c r="Q36" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="R30" s="9" t="s">
+      <c r="R36" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="S30" s="9" t="s">
+      <c r="S36" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C31" s="10" t="str">
+    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C37" s="10" t="str">
         <f>D18</f>
         <v>Supply Labour-Primary</v>
       </c>
-      <c r="D31" s="10" t="str">
+      <c r="D37" s="10" t="str">
         <f>C18</f>
         <v>MINFLAB-P</v>
       </c>
-      <c r="E31" s="11" t="str">
+      <c r="E37" s="11" t="str">
         <f>C5</f>
         <v>FLAB-P</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="J31" s="10" t="str">
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="J37" s="10" t="str">
         <f>K18</f>
         <v>Supply Construction</v>
       </c>
-      <c r="K31" s="10" t="str">
+      <c r="K37" s="10" t="str">
         <f>J18</f>
         <v>MINccons_e</v>
       </c>
-      <c r="L31" s="11" t="str">
+      <c r="L37" s="11" t="str">
         <f>J5</f>
         <v>ccons_e</v>
       </c>
-      <c r="Q31" s="10" t="str">
+      <c r="Q37" s="10" t="str">
         <f>R18</f>
         <v>Supply Material - Steel</v>
       </c>
-      <c r="R31" s="10" t="str">
+      <c r="R37" s="10" t="str">
         <f>Q18</f>
         <v>MINMATSTL</v>
       </c>
-      <c r="S31" s="11" t="str">
+      <c r="S37" s="11" t="str">
         <f>Q5</f>
         <v>MATSTL</v>
       </c>
     </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C32" s="10" t="str">
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C38" s="10" t="str">
         <f>D19</f>
         <v>Supply Labour-Mid</v>
       </c>
-      <c r="D32" s="10" t="str">
+      <c r="D38" s="10" t="str">
         <f>C19</f>
         <v>MINFLAB-M</v>
       </c>
-      <c r="E32" s="11" t="str">
+      <c r="E38" s="11" t="str">
         <f>C6</f>
         <v>FLAB-M</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="J32" s="10" t="str">
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="J38" s="10" t="str">
         <f>K19</f>
         <v>Supply Machinery</v>
       </c>
-      <c r="K32" s="10" t="str">
+      <c r="K38" s="10" t="str">
         <f>J19</f>
         <v>MINcmach_e</v>
       </c>
-      <c r="L32" s="11" t="str">
+      <c r="L38" s="11" t="str">
         <f>J6</f>
         <v>cmach_e</v>
       </c>
-      <c r="Q32" s="10" t="str">
-        <f t="shared" ref="Q32:Q40" si="2">R19</f>
+      <c r="Q38" s="10" t="str">
+        <f t="shared" ref="Q38:Q46" si="9">R19</f>
         <v>Supply Material - Aluminium</v>
       </c>
-      <c r="R32" s="10" t="str">
-        <f t="shared" ref="R32:R40" si="3">Q19</f>
+      <c r="R38" s="10" t="str">
+        <f t="shared" ref="R38:R46" si="10">Q19</f>
         <v>MINMATALU</v>
       </c>
-      <c r="S32" s="11" t="str">
-        <f t="shared" ref="S32:S38" si="4">Q6</f>
+      <c r="S38" s="11" t="str">
+        <f t="shared" ref="S38:S44" si="11">Q6</f>
         <v>MATALU</v>
       </c>
     </row>
-    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C33" s="10" t="str">
+    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C39" s="10" t="str">
         <f>D20</f>
         <v>Supply Labour-Secondary</v>
       </c>
-      <c r="D33" s="10" t="str">
+      <c r="D39" s="10" t="str">
         <f>C20</f>
         <v>MINFLAB-S</v>
       </c>
-      <c r="E33" s="11" t="str">
+      <c r="E39" s="11" t="str">
         <f>C7</f>
         <v>FLAB-S</v>
       </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="J33" s="10" t="str">
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="J39" s="10" t="str">
         <f>K20</f>
         <v>Supply Electrical Machinery</v>
       </c>
-      <c r="K33" s="10" t="str">
+      <c r="K39" s="10" t="str">
         <f>J20</f>
         <v>MINcemch_e</v>
       </c>
-      <c r="L33" s="11" t="str">
+      <c r="L39" s="11" t="str">
         <f>J7</f>
         <v>cemch_e</v>
       </c>
-      <c r="Q33" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q39" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>Supply Material - Cement</v>
       </c>
-      <c r="R33" s="10" t="str">
-        <f t="shared" si="3"/>
+      <c r="R39" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>MINMATCEM</v>
       </c>
-      <c r="S33" s="11" t="str">
-        <f t="shared" si="4"/>
+      <c r="S39" s="11" t="str">
+        <f t="shared" si="11"/>
         <v>MATCEM</v>
       </c>
     </row>
-    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C34" s="10" t="str">
+    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C40" s="10" t="str">
         <f>D21</f>
         <v>Supply Labour-Tertiary</v>
       </c>
-      <c r="D34" s="10" t="str">
+      <c r="D40" s="10" t="str">
         <f>C21</f>
         <v>MINFLAB-T</v>
       </c>
-      <c r="E34" s="11" t="str">
+      <c r="E40" s="11" t="str">
         <f>C8</f>
         <v>FLAB-T</v>
       </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="J34" s="10" t="str">
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="J40" s="10" t="str">
         <f>K21</f>
         <v>Supply Metal Products</v>
       </c>
-      <c r="K34" s="10" t="str">
+      <c r="K40" s="10" t="str">
         <f>J21</f>
         <v>MINcmetp</v>
       </c>
-      <c r="L34" s="11" t="str">
+      <c r="L40" s="11" t="str">
         <f>J8</f>
         <v>cmetp</v>
       </c>
-      <c r="Q34" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q40" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>Supply Material - Plastic</v>
       </c>
-      <c r="R34" s="10" t="str">
-        <f t="shared" si="3"/>
+      <c r="R40" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>MINMATPLT</v>
       </c>
-      <c r="S34" s="11" t="str">
-        <f t="shared" si="4"/>
+      <c r="S40" s="11" t="str">
+        <f t="shared" si="11"/>
         <v>MATPLT</v>
       </c>
     </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="3"/>
-      <c r="J35" s="10" t="str">
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="3"/>
+      <c r="J41" s="10" t="str">
         <f>K22</f>
         <v>Supply Business Services</v>
       </c>
-      <c r="K35" s="10" t="str">
+      <c r="K41" s="10" t="str">
         <f>J22</f>
         <v>MINcbsrv</v>
       </c>
-      <c r="L35" s="11" t="str">
+      <c r="L41" s="11" t="str">
         <f>J9</f>
         <v>cbsrv</v>
       </c>
-      <c r="Q35" s="10" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q41" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>Supply Material - Glass</v>
       </c>
-      <c r="R35" s="10" t="str">
-        <f t="shared" si="3"/>
+      <c r="R41" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>MINMATGLS</v>
       </c>
-      <c r="S35" s="11" t="str">
-        <f t="shared" si="4"/>
+      <c r="S41" s="11" t="str">
+        <f t="shared" si="11"/>
         <v>MATGLS</v>
       </c>
     </row>
-    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="3"/>
-      <c r="Q36" s="10" t="str">
-        <f t="shared" si="2"/>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="3"/>
+      <c r="J42" s="10" t="str">
+        <f>K23</f>
+        <v>Imports of Construction</v>
+      </c>
+      <c r="K42" s="10" t="str">
+        <f>J23</f>
+        <v>IMPccons_e</v>
+      </c>
+      <c r="L42" s="15" t="str">
+        <f>J5</f>
+        <v>ccons_e</v>
+      </c>
+      <c r="Q42" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>Supply Material - Copper</v>
       </c>
-      <c r="R36" s="10" t="str">
-        <f t="shared" si="3"/>
+      <c r="R42" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>MINMATCOP</v>
       </c>
-      <c r="S36" s="11" t="str">
-        <f t="shared" si="4"/>
+      <c r="S42" s="11" t="str">
+        <f t="shared" si="11"/>
         <v>MATCOP</v>
       </c>
     </row>
-    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="Q37" s="10" t="str">
-        <f t="shared" si="2"/>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="J43" s="10" t="str">
+        <f t="shared" ref="J43:J47" si="12">K24</f>
+        <v>Imports of Machinery</v>
+      </c>
+      <c r="K43" s="10" t="str">
+        <f t="shared" ref="K43:K47" si="13">J24</f>
+        <v>IMPcmach_e</v>
+      </c>
+      <c r="L43" s="15" t="str">
+        <f t="shared" ref="L43:L47" si="14">J6</f>
+        <v>cmach_e</v>
+      </c>
+      <c r="Q43" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>Supply Material - Nickel</v>
       </c>
-      <c r="R37" s="10" t="str">
-        <f t="shared" si="3"/>
+      <c r="R43" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>MINMATNIC</v>
       </c>
-      <c r="S37" s="11" t="str">
-        <f t="shared" si="4"/>
+      <c r="S43" s="11" t="str">
+        <f t="shared" si="11"/>
         <v>MATNIC</v>
       </c>
     </row>
-    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="Q38" s="10" t="str">
-        <f t="shared" si="2"/>
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="J44" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>Imports of Electrical Machinery</v>
+      </c>
+      <c r="K44" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>IMPcemch_e</v>
+      </c>
+      <c r="L44" s="15" t="str">
+        <f t="shared" si="14"/>
+        <v>cemch_e</v>
+      </c>
+      <c r="Q44" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>Supply Material - Manganese</v>
       </c>
-      <c r="R38" s="10" t="str">
-        <f t="shared" si="3"/>
+      <c r="R44" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>MINMATMNG</v>
       </c>
-      <c r="S38" s="11" t="str">
-        <f t="shared" si="4"/>
+      <c r="S44" s="11" t="str">
+        <f t="shared" si="11"/>
         <v>MATMNG</v>
       </c>
     </row>
-    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="Q39" s="10" t="str">
+    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="J45" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>Imports of Metal Products</v>
+      </c>
+      <c r="K45" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>IMPcmetp</v>
+      </c>
+      <c r="L45" s="15" t="str">
+        <f t="shared" si="14"/>
+        <v>cmetp</v>
+      </c>
+      <c r="Q45" s="10" t="str">
         <f>R26</f>
         <v>Supply Material - Cobalt</v>
       </c>
-      <c r="R39" s="10" t="str">
+      <c r="R45" s="10" t="str">
         <f>Q26</f>
         <v>MINMATCOB</v>
       </c>
-      <c r="S39" s="11" t="str">
+      <c r="S45" s="11" t="str">
         <f>Q13</f>
         <v>MATCOB</v>
       </c>
     </row>
-    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="Q40" s="10" t="str">
-        <f t="shared" si="2"/>
+    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="J46" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>Imports of Business Services</v>
+      </c>
+      <c r="K46" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v>IMPcbsrv</v>
+      </c>
+      <c r="L46" s="15" t="str">
+        <f t="shared" si="14"/>
+        <v>cbsrv</v>
+      </c>
+      <c r="Q46" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>Supply Material - Silicon</v>
       </c>
-      <c r="R40" s="10" t="str">
-        <f t="shared" si="3"/>
+      <c r="R46" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>MINMATSIL</v>
       </c>
-      <c r="S40" s="11" t="str">
-        <f t="shared" ref="S40" si="5">Q14</f>
+      <c r="S46" s="11" t="str">
+        <f t="shared" ref="S46" si="15">Q14</f>
         <v>MATSIL</v>
       </c>
     </row>
+    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="15"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AL26:AM60">
-    <sortCondition descending="1" ref="AM26:AM60"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AL26:AM66">
+    <sortCondition descending="1" ref="AM26:AM66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>